<commit_message>
Export CSV Data works now
</commit_message>
<xml_diff>
--- a/specification/TourPlanner_Checklist_Final.xlsx
+++ b/specification/TourPlanner_Checklist_Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wermann\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsnyr/Documents/Documents - Baris’s MacBook Pro/02FHLocal/04Semester/SWEN2/MBTourPlanner/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588BFEB6-2911-4B5E-ADF7-5FC033BC1175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9C32E4-1559-5D47-82F6-00E1A174C047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17496" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -340,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -353,10 +353,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -390,9 +389,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -430,7 +429,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -536,7 +535,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -688,44 +687,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="170" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="70.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="104.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="104.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
@@ -733,18 +732,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>1</v>
       </c>
@@ -752,7 +751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>2</v>
       </c>
@@ -760,7 +759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>3</v>
       </c>
@@ -768,7 +767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
@@ -776,7 +775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>5</v>
       </c>
@@ -784,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
@@ -792,7 +791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>54</v>
       </c>
@@ -800,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>6</v>
       </c>
@@ -808,7 +807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>60</v>
       </c>
@@ -816,7 +815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>9</v>
       </c>
@@ -824,7 +823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>10</v>
       </c>
@@ -832,7 +831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>7</v>
       </c>
@@ -840,12 +839,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>12</v>
       </c>
@@ -856,39 +855,39 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="31" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>64</v>
       </c>
@@ -896,14 +895,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="6"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>49</v>
       </c>
@@ -912,7 +911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>66</v>
       </c>
@@ -920,19 +919,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="6"/>
     </row>
-    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>65</v>
       </c>
@@ -940,14 +939,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="6"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>46</v>
       </c>
@@ -955,21 +954,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="6"/>
     </row>
-    <row r="44" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B44"/>
       <c r="C44"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>55</v>
       </c>
@@ -977,7 +976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>17</v>
       </c>
@@ -985,14 +984,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B48"/>
       <c r="C48"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>34</v>
       </c>
@@ -1000,7 +999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>20</v>
       </c>
@@ -1008,7 +1007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>18</v>
       </c>
@@ -1016,7 +1015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>19</v>
       </c>
@@ -1024,7 +1023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -1032,14 +1031,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B56"/>
       <c r="C56"/>
     </row>
-    <row r="57" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>28</v>
       </c>
@@ -1047,7 +1046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>31</v>
       </c>
@@ -1055,7 +1054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>61</v>
       </c>
@@ -1063,7 +1062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>62</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>48</v>
       </c>
@@ -1079,7 +1078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>44</v>
       </c>
@@ -1087,7 +1086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>32</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>47</v>
       </c>
@@ -1103,14 +1102,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>56</v>
       </c>
@@ -1118,7 +1117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>59</v>
       </c>
@@ -1126,14 +1125,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B70" s="10"/>
       <c r="C70" s="6"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>57</v>
       </c>
@@ -1141,7 +1140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>23</v>
       </c>
@@ -1149,7 +1148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
         <v>24</v>
       </c>
@@ -1157,7 +1156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
         <v>25</v>
       </c>
@@ -1165,7 +1164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
         <v>27</v>
       </c>
@@ -1173,7 +1172,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>51</v>
       </c>
@@ -1181,14 +1180,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B78"/>
       <c r="C78" s="6"/>
     </row>
-    <row r="80" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
tour-report is optimized, image still not visible, but logic kinda implemented
</commit_message>
<xml_diff>
--- a/specification/TourPlanner_Checklist_Final.xlsx
+++ b/specification/TourPlanner_Checklist_Final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsnyr/Documents/Documents - Baris’s MacBook Pro/02FHLocal/04Semester/SWEN2/MBTourPlanner/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9C32E4-1559-5D47-82F6-00E1A174C047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716E2836-4672-954E-B793-768F90788374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
+    <workbookView xWindow="4440" yWindow="880" windowWidth="31560" windowHeight="21080" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -687,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="170" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="200" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>